<commit_message>
Update start year for buildings files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
+++ b/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\India\India_Model\InputData\bldgs\SYCEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\bldgs\SYCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF25953-F2F8-4732-B4D3-084ED492C00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21150" yWindow="2250" windowWidth="20655" windowHeight="12825" tabRatio="776" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-28680" yWindow="2160" windowWidth="15480" windowHeight="12375" activeTab="1" xr2:uid="{CB934753-F4B4-4DB1-82B7-5ADC08BBD442}"/>
+    <workbookView xWindow="-21150" yWindow="2250" windowWidth="20655" windowHeight="12825" tabRatio="776"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +18,7 @@
     <sheet name="SYCEU-rural-residential" sheetId="30" r:id="rId4"/>
     <sheet name="SYCEU-commercial" sheetId="31" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -226,9 +224,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -485,7 +483,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -500,23 +498,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Header: top rows" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Body: normal cell 2" xfId="11"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="13"/>
+    <cellStyle name="Footnotes: top row" xfId="6"/>
+    <cellStyle name="Footnotes: top row 2" xfId="9"/>
+    <cellStyle name="Header: bottom row" xfId="2"/>
+    <cellStyle name="Header: bottom row 2" xfId="12"/>
+    <cellStyle name="Header: top rows" xfId="16"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Parent row 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="8"/>
+    <cellStyle name="Parent row" xfId="5"/>
+    <cellStyle name="Parent row 2" xfId="10"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Table title" xfId="3" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Table title 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Table title" xfId="3"/>
+    <cellStyle name="Table title 2" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -607,23 +605,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -659,23 +640,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -851,13 +815,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1041,7 +1004,7 @@
     </row>
     <row r="41" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="10">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -1168,7 +1131,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" xr:uid="{B33A1742-5615-419B-9D33-AA6AC4954902}"/>
+    <hyperlink ref="B35" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -1176,17 +1139,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED24824-075F-4B47-8D62-4734D7DE2FE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:AK151"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="1">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:AK151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18265,21 +18225,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M41" sqref="M41"/>
       <selection pane="topRight" activeCell="M41" sqref="M41"/>
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18323,7 +18280,7 @@
       </c>
       <c r="C2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,C$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>74230285047056.813</v>
+        <v>91643082695721.781</v>
       </c>
       <c r="D2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,D$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
@@ -18331,15 +18288,15 @@
       </c>
       <c r="E2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,E$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>54075037063113.539</v>
+        <v>57766719469841.469</v>
       </c>
       <c r="F2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>149920662784308.41</v>
+        <v>167016388205793.28</v>
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>29793011115519.977</v>
+        <v>35404039443898.594</v>
       </c>
       <c r="I2" s="8"/>
     </row>
@@ -18394,7 +18351,7 @@
       </c>
       <c r="F4" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A4)</f>
-        <v>74865213239966.547</v>
+        <v>83736758498055.078</v>
       </c>
       <c r="G4" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A4)</f>
@@ -18481,7 +18438,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A7)</f>
-        <v>467225402671796.38</v>
+        <v>447563177736256.06</v>
       </c>
       <c r="G7" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A7)</f>
@@ -18568,7 +18525,7 @@
       </c>
       <c r="F10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>
-        <v>598966165903575.75</v>
+        <v>613594869391822.25</v>
       </c>
       <c r="G10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Urban Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>
@@ -18611,7 +18568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C363CC6-2AF1-40D2-9144-7FE415EBF2FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -18624,7 +18581,6 @@
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -18663,11 +18619,11 @@
       </c>
       <c r="B2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,B$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,C$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>150709972671298.06</v>
+        <v>180699697898432.28</v>
       </c>
       <c r="D2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,D$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
@@ -18675,15 +18631,15 @@
       </c>
       <c r="E2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,E$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>109788711612988.75</v>
+        <v>113903073202393.92</v>
       </c>
       <c r="F2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>304384375956021.94</v>
+        <v>329319027744611.56</v>
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>60488840749692.438</v>
+        <v>69808861113260.156</v>
       </c>
       <c r="I2" s="8"/>
     </row>
@@ -18738,7 +18694,7 @@
       </c>
       <c r="F4" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A4)</f>
-        <v>30861817111245.664</v>
+        <v>34489590862747.207</v>
       </c>
       <c r="G4" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A4)</f>
@@ -18825,7 +18781,7 @@
       </c>
       <c r="F7" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A7)</f>
-        <v>3808536069842086.5</v>
+        <v>3612497415464614</v>
       </c>
       <c r="G7" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A7)</f>
@@ -18850,11 +18806,11 @@
       </c>
       <c r="E8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,E$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
-        <v>135916322988352.5</v>
+        <v>108733058390682</v>
       </c>
       <c r="F8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
-        <v>15101813665372.5</v>
+        <v>12081450932298</v>
       </c>
       <c r="G8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
@@ -18912,7 +18868,7 @@
       </c>
       <c r="F10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>
-        <v>313037451949964.38</v>
+        <v>336891349652692.69</v>
       </c>
       <c r="G10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Rural Residential",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>
@@ -18955,7 +18911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC05FCB0-8DA3-4DD4-BAD8-E7EDBDA67910}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -18968,7 +18924,6 @@
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
       <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -19011,7 +18966,7 @@
       </c>
       <c r="C2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,C$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>188023039078421.66</v>
+        <v>201033808519699.41</v>
       </c>
       <c r="D2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,D$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
@@ -19019,15 +18974,15 @@
       </c>
       <c r="E2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,E$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>43081261657360.836</v>
+        <v>44985202764349.727</v>
       </c>
       <c r="F2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>62639988008697.188</v>
+        <v>64730113102559.594</v>
       </c>
       <c r="G2" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A2)</f>
-        <v>34302262995520.332</v>
+        <v>36463019416576.25</v>
       </c>
       <c r="I2" s="8"/>
     </row>
@@ -19194,11 +19149,11 @@
       </c>
       <c r="E8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,E$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
-        <v>3215758233897</v>
+        <v>2572606587117.6001</v>
       </c>
       <c r="F8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
-        <v>357306470433</v>
+        <v>285845176346.40002</v>
       </c>
       <c r="G8" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A8)</f>
@@ -19256,7 +19211,7 @@
       </c>
       <c r="F10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,F$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>
-        <v>93462295881150</v>
+        <v>97405999818698.172</v>
       </c>
       <c r="G10" s="13">
         <f>SUMIFS(INDEX('Calculations - from BCEU'!$D$2:$AK$151,,MATCH(About!$A$41,'Calculations - from BCEU'!$D$1:$AK$1,0)),'Calculations - from BCEU'!$A$2:$A$151,"Commercial",'Calculations - from BCEU'!$C$2:$C$151,G$1,'Calculations - from BCEU'!$B$2:$B$151,$A10)</f>

</xml_diff>